<commit_message>
Initial deployment of Azure VMs from Excel
</commit_message>
<xml_diff>
--- a/Create-AzVmsFromExcel/Azure Virtual Machine Configuration.xlsx
+++ b/Create-AzVmsFromExcel/Azure Virtual Machine Configuration.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
   <si>
     <t>Subnet</t>
   </si>
@@ -174,6 +174,15 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>jf-rg-001</t>
+  </si>
+  <si>
+    <t>jf-vm-001</t>
+  </si>
+  <si>
+    <t>jf-vm-001754</t>
   </si>
 </sst>
 </file>
@@ -543,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AH3" sqref="AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -735,11 +744,65 @@
         <v>127</v>
       </c>
     </row>
+    <row r="3" spans="1:32" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" t="s">
+        <v>50</v>
+      </c>
+      <c r="W3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>